<commit_message>
balance and benford check done
</commit_message>
<xml_diff>
--- a/Liushui/output/output2.xlsx
+++ b/Liushui/output/output2.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt formatCode="yyyy-mm-dd" numFmtId="164"/>
+    <numFmt formatCode="YYYY-MM-DD" numFmtId="165"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -56,11 +59,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -437,8 +441,8 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
-        <v>20190202</v>
+      <c r="B2" s="2" t="n">
+        <v>43498</v>
       </c>
       <c r="C2" t="n">
         <v>41850</v>
@@ -481,8 +485,8 @@
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
-        <v>20190202</v>
+      <c r="B3" s="2" t="n">
+        <v>43498</v>
       </c>
       <c r="C3" t="n">
         <v>42731</v>
@@ -525,8 +529,8 @@
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="n">
-        <v>20190202</v>
+      <c r="B4" s="2" t="n">
+        <v>43498</v>
       </c>
       <c r="C4" t="n">
         <v>44954</v>
@@ -569,8 +573,8 @@
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="n">
-        <v>20190212</v>
+      <c r="B5" s="2" t="n">
+        <v>43508</v>
       </c>
       <c r="C5" t="n">
         <v>2940</v>
@@ -613,8 +617,8 @@
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="n">
-        <v>20190213</v>
+      <c r="B6" s="2" t="n">
+        <v>43509</v>
       </c>
       <c r="C6" t="n">
         <v>100651</v>
@@ -657,8 +661,8 @@
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="n">
-        <v>20190213</v>
+      <c r="B7" s="2" t="n">
+        <v>43509</v>
       </c>
       <c r="C7" t="n">
         <v>173930</v>
@@ -709,8 +713,8 @@
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" t="n">
-        <v>20190215</v>
+      <c r="B8" s="2" t="n">
+        <v>43511</v>
       </c>
       <c r="C8" t="n">
         <v>95357</v>
@@ -757,8 +761,8 @@
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" t="n">
-        <v>20190302</v>
+      <c r="B9" s="2" t="n">
+        <v>43526</v>
       </c>
       <c r="C9" t="n">
         <v>40827</v>
@@ -801,8 +805,8 @@
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" t="n">
-        <v>20190302</v>
+      <c r="B10" s="2" t="n">
+        <v>43526</v>
       </c>
       <c r="C10" t="n">
         <v>44407</v>
@@ -845,8 +849,8 @@
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" t="n">
-        <v>20190311</v>
+      <c r="B11" s="2" t="n">
+        <v>43535</v>
       </c>
       <c r="C11" t="n">
         <v>145132</v>
@@ -897,8 +901,8 @@
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12" t="n">
-        <v>20190311</v>
+      <c r="B12" s="2" t="n">
+        <v>43535</v>
       </c>
       <c r="C12" t="n">
         <v>145132</v>
@@ -949,8 +953,8 @@
       <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B13" t="n">
-        <v>20190311</v>
+      <c r="B13" s="2" t="n">
+        <v>43535</v>
       </c>
       <c r="C13" t="n">
         <v>145132</v>
@@ -1001,8 +1005,8 @@
       <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B14" t="n">
-        <v>20190311</v>
+      <c r="B14" s="2" t="n">
+        <v>43535</v>
       </c>
       <c r="C14" t="n">
         <v>145132</v>
@@ -1053,8 +1057,8 @@
       <c r="A15" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B15" t="n">
-        <v>20190311</v>
+      <c r="B15" s="2" t="n">
+        <v>43535</v>
       </c>
       <c r="C15" t="n">
         <v>145132</v>
@@ -1105,8 +1109,8 @@
       <c r="A16" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B16" t="n">
-        <v>20190311</v>
+      <c r="B16" s="2" t="n">
+        <v>43535</v>
       </c>
       <c r="C16" t="n">
         <v>145132</v>
@@ -1157,8 +1161,8 @@
       <c r="A17" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B17" t="n">
-        <v>20190311</v>
+      <c r="B17" s="2" t="n">
+        <v>43535</v>
       </c>
       <c r="C17" t="n">
         <v>145132</v>
@@ -1209,8 +1213,8 @@
       <c r="A18" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B18" t="n">
-        <v>20190311</v>
+      <c r="B18" s="2" t="n">
+        <v>43535</v>
       </c>
       <c r="C18" t="n">
         <v>145132</v>
@@ -1261,8 +1265,8 @@
       <c r="A19" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B19" t="n">
-        <v>20190311</v>
+      <c r="B19" s="2" t="n">
+        <v>43535</v>
       </c>
       <c r="C19" t="n">
         <v>145133</v>
@@ -1313,8 +1317,8 @@
       <c r="A20" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B20" t="n">
-        <v>20190312</v>
+      <c r="B20" s="2" t="n">
+        <v>43536</v>
       </c>
       <c r="C20" t="n">
         <v>436</v>
@@ -1357,8 +1361,8 @@
       <c r="A21" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B21" t="n">
-        <v>20190312</v>
+      <c r="B21" s="2" t="n">
+        <v>43536</v>
       </c>
       <c r="C21" t="n">
         <v>105519</v>
@@ -1405,8 +1409,8 @@
       <c r="A22" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B22" t="n">
-        <v>20190314</v>
+      <c r="B22" s="2" t="n">
+        <v>43538</v>
       </c>
       <c r="C22" t="n">
         <v>83108</v>
@@ -1457,8 +1461,8 @@
       <c r="A23" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B23" t="n">
-        <v>20190314</v>
+      <c r="B23" s="2" t="n">
+        <v>43538</v>
       </c>
       <c r="C23" t="n">
         <v>94147</v>
@@ -1509,8 +1513,8 @@
       <c r="A24" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B24" t="n">
-        <v>20190314</v>
+      <c r="B24" s="2" t="n">
+        <v>43538</v>
       </c>
       <c r="C24" t="n">
         <v>95829</v>
@@ -1553,8 +1557,8 @@
       <c r="A25" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B25" t="n">
-        <v>20190318</v>
+      <c r="B25" s="2" t="n">
+        <v>43542</v>
       </c>
       <c r="C25" t="n">
         <v>152246</v>
@@ -1605,8 +1609,8 @@
       <c r="A26" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="B26" t="n">
-        <v>20190319</v>
+      <c r="B26" s="2" t="n">
+        <v>43543</v>
       </c>
       <c r="C26" t="n">
         <v>210337</v>
@@ -1657,8 +1661,8 @@
       <c r="A27" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="B27" t="n">
-        <v>20190320</v>
+      <c r="B27" s="2" t="n">
+        <v>43544</v>
       </c>
       <c r="C27" t="n">
         <v>144221</v>
@@ -1705,8 +1709,8 @@
       <c r="A28" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="B28" t="n">
-        <v>20190321</v>
+      <c r="B28" s="2" t="n">
+        <v>43545</v>
       </c>
       <c r="C28" t="n">
         <v>22303</v>
@@ -1749,8 +1753,8 @@
       <c r="A29" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="B29" t="n">
-        <v>20190321</v>
+      <c r="B29" s="2" t="n">
+        <v>43545</v>
       </c>
       <c r="C29" t="n">
         <v>113113</v>
@@ -1801,8 +1805,8 @@
       <c r="A30" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="B30" t="n">
-        <v>20190321</v>
+      <c r="B30" s="2" t="n">
+        <v>43545</v>
       </c>
       <c r="C30" t="n">
         <v>113113</v>
@@ -1853,8 +1857,8 @@
       <c r="A31" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="B31" t="n">
-        <v>20190321</v>
+      <c r="B31" s="2" t="n">
+        <v>43545</v>
       </c>
       <c r="C31" t="n">
         <v>113113</v>
@@ -1905,8 +1909,8 @@
       <c r="A32" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="B32" t="n">
-        <v>20190321</v>
+      <c r="B32" s="2" t="n">
+        <v>43545</v>
       </c>
       <c r="C32" t="n">
         <v>113113</v>
@@ -1957,8 +1961,8 @@
       <c r="A33" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="B33" t="n">
-        <v>20190321</v>
+      <c r="B33" s="2" t="n">
+        <v>43545</v>
       </c>
       <c r="C33" t="n">
         <v>113113</v>
@@ -2009,8 +2013,8 @@
       <c r="A34" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B34" t="n">
-        <v>20190321</v>
+      <c r="B34" s="2" t="n">
+        <v>43545</v>
       </c>
       <c r="C34" t="n">
         <v>113113</v>
@@ -2061,8 +2065,8 @@
       <c r="A35" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="B35" t="n">
-        <v>20190321</v>
+      <c r="B35" s="2" t="n">
+        <v>43545</v>
       </c>
       <c r="C35" t="n">
         <v>113113</v>
@@ -2113,8 +2117,8 @@
       <c r="A36" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="B36" t="n">
-        <v>20190321</v>
+      <c r="B36" s="2" t="n">
+        <v>43545</v>
       </c>
       <c r="C36" t="n">
         <v>113113</v>
@@ -2165,8 +2169,8 @@
       <c r="A37" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="B37" t="n">
-        <v>20190321</v>
+      <c r="B37" s="2" t="n">
+        <v>43545</v>
       </c>
       <c r="C37" t="n">
         <v>165109</v>
@@ -2217,8 +2221,8 @@
       <c r="A38" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="B38" t="n">
-        <v>20190402</v>
+      <c r="B38" s="2" t="n">
+        <v>43557</v>
       </c>
       <c r="C38" t="n">
         <v>43040</v>
@@ -2261,8 +2265,8 @@
       <c r="A39" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="B39" t="n">
-        <v>20190402</v>
+      <c r="B39" s="2" t="n">
+        <v>43557</v>
       </c>
       <c r="C39" t="n">
         <v>43040</v>
@@ -2305,8 +2309,8 @@
       <c r="A40" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="B40" t="n">
-        <v>20190402</v>
+      <c r="B40" s="2" t="n">
+        <v>43557</v>
       </c>
       <c r="C40" t="n">
         <v>44343</v>
@@ -2349,8 +2353,8 @@
       <c r="A41" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="B41" t="n">
-        <v>20190408</v>
+      <c r="B41" s="2" t="n">
+        <v>43563</v>
       </c>
       <c r="C41" t="n">
         <v>102804</v>
@@ -2397,8 +2401,8 @@
       <c r="A42" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="B42" t="n">
-        <v>20190408</v>
+      <c r="B42" s="2" t="n">
+        <v>43563</v>
       </c>
       <c r="C42" t="n">
         <v>113435</v>
@@ -2441,8 +2445,8 @@
       <c r="A43" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="B43" t="n">
-        <v>20190408</v>
+      <c r="B43" s="2" t="n">
+        <v>43563</v>
       </c>
       <c r="C43" t="n">
         <v>114530</v>
@@ -2489,8 +2493,8 @@
       <c r="A44" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="B44" t="n">
-        <v>20190410</v>
+      <c r="B44" s="2" t="n">
+        <v>43565</v>
       </c>
       <c r="C44" t="n">
         <v>113709</v>
@@ -2541,8 +2545,8 @@
       <c r="A45" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="B45" t="n">
-        <v>20190410</v>
+      <c r="B45" s="2" t="n">
+        <v>43565</v>
       </c>
       <c r="C45" t="n">
         <v>113709</v>
@@ -2593,8 +2597,8 @@
       <c r="A46" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="B46" t="n">
-        <v>20190410</v>
+      <c r="B46" s="2" t="n">
+        <v>43565</v>
       </c>
       <c r="C46" t="n">
         <v>113709</v>
@@ -2645,8 +2649,8 @@
       <c r="A47" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="B47" t="n">
-        <v>20190410</v>
+      <c r="B47" s="2" t="n">
+        <v>43565</v>
       </c>
       <c r="C47" t="n">
         <v>113709</v>
@@ -2697,8 +2701,8 @@
       <c r="A48" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="B48" t="n">
-        <v>20190410</v>
+      <c r="B48" s="2" t="n">
+        <v>43565</v>
       </c>
       <c r="C48" t="n">
         <v>113709</v>
@@ -2749,8 +2753,8 @@
       <c r="A49" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="B49" t="n">
-        <v>20190410</v>
+      <c r="B49" s="2" t="n">
+        <v>43565</v>
       </c>
       <c r="C49" t="n">
         <v>113709</v>
@@ -2801,8 +2805,8 @@
       <c r="A50" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="B50" t="n">
-        <v>20190410</v>
+      <c r="B50" s="2" t="n">
+        <v>43565</v>
       </c>
       <c r="C50" t="n">
         <v>113709</v>
@@ -2853,8 +2857,8 @@
       <c r="A51" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="B51" t="n">
-        <v>20190410</v>
+      <c r="B51" s="2" t="n">
+        <v>43565</v>
       </c>
       <c r="C51" t="n">
         <v>113709</v>
@@ -2905,8 +2909,8 @@
       <c r="A52" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="B52" t="n">
-        <v>20190410</v>
+      <c r="B52" s="2" t="n">
+        <v>43565</v>
       </c>
       <c r="C52" t="n">
         <v>113709</v>
@@ -2957,8 +2961,8 @@
       <c r="A53" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="B53" t="n">
-        <v>20190410</v>
+      <c r="B53" s="2" t="n">
+        <v>43565</v>
       </c>
       <c r="C53" t="n">
         <v>113709</v>
@@ -3009,8 +3013,8 @@
       <c r="A54" s="1" t="n">
         <v>52</v>
       </c>
-      <c r="B54" t="n">
-        <v>20190411</v>
+      <c r="B54" s="2" t="n">
+        <v>43566</v>
       </c>
       <c r="C54" t="n">
         <v>4740</v>
@@ -3053,8 +3057,8 @@
       <c r="A55" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="B55" t="n">
-        <v>20190502</v>
+      <c r="B55" s="2" t="n">
+        <v>43587</v>
       </c>
       <c r="C55" t="n">
         <v>45752</v>
@@ -3097,8 +3101,8 @@
       <c r="A56" s="1" t="n">
         <v>54</v>
       </c>
-      <c r="B56" t="n">
-        <v>20190502</v>
+      <c r="B56" s="2" t="n">
+        <v>43587</v>
       </c>
       <c r="C56" t="n">
         <v>54349</v>
@@ -3141,8 +3145,8 @@
       <c r="A57" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="B57" t="n">
-        <v>20190502</v>
+      <c r="B57" s="2" t="n">
+        <v>43587</v>
       </c>
       <c r="C57" t="n">
         <v>54349</v>
@@ -3185,8 +3189,8 @@
       <c r="A58" s="1" t="n">
         <v>56</v>
       </c>
-      <c r="B58" t="n">
-        <v>20190508</v>
+      <c r="B58" s="2" t="n">
+        <v>43593</v>
       </c>
       <c r="C58" t="n">
         <v>103430</v>
@@ -3233,8 +3237,8 @@
       <c r="A59" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="B59" t="n">
-        <v>20190510</v>
+      <c r="B59" s="2" t="n">
+        <v>43595</v>
       </c>
       <c r="C59" t="n">
         <v>95256</v>
@@ -3285,8 +3289,8 @@
       <c r="A60" s="1" t="n">
         <v>58</v>
       </c>
-      <c r="B60" t="n">
-        <v>20190510</v>
+      <c r="B60" s="2" t="n">
+        <v>43595</v>
       </c>
       <c r="C60" t="n">
         <v>105155</v>
@@ -3329,8 +3333,8 @@
       <c r="A61" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="B61" t="n">
-        <v>20190510</v>
+      <c r="B61" s="2" t="n">
+        <v>43595</v>
       </c>
       <c r="C61" t="n">
         <v>110405</v>
@@ -3377,8 +3381,8 @@
       <c r="A62" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="B62" t="n">
-        <v>20190510</v>
+      <c r="B62" s="2" t="n">
+        <v>43595</v>
       </c>
       <c r="C62" t="n">
         <v>112529</v>
@@ -3429,8 +3433,8 @@
       <c r="A63" s="1" t="n">
         <v>61</v>
       </c>
-      <c r="B63" t="n">
-        <v>20190510</v>
+      <c r="B63" s="2" t="n">
+        <v>43595</v>
       </c>
       <c r="C63" t="n">
         <v>112529</v>
@@ -3481,8 +3485,8 @@
       <c r="A64" s="1" t="n">
         <v>62</v>
       </c>
-      <c r="B64" t="n">
-        <v>20190510</v>
+      <c r="B64" s="2" t="n">
+        <v>43595</v>
       </c>
       <c r="C64" t="n">
         <v>112530</v>
@@ -3533,8 +3537,8 @@
       <c r="A65" s="1" t="n">
         <v>63</v>
       </c>
-      <c r="B65" t="n">
-        <v>20190510</v>
+      <c r="B65" s="2" t="n">
+        <v>43595</v>
       </c>
       <c r="C65" t="n">
         <v>112530</v>
@@ -3585,8 +3589,8 @@
       <c r="A66" s="1" t="n">
         <v>64</v>
       </c>
-      <c r="B66" t="n">
-        <v>20190510</v>
+      <c r="B66" s="2" t="n">
+        <v>43595</v>
       </c>
       <c r="C66" t="n">
         <v>112530</v>
@@ -3637,8 +3641,8 @@
       <c r="A67" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="B67" t="n">
-        <v>20190510</v>
+      <c r="B67" s="2" t="n">
+        <v>43595</v>
       </c>
       <c r="C67" t="n">
         <v>112530</v>
@@ -3689,8 +3693,8 @@
       <c r="A68" s="1" t="n">
         <v>66</v>
       </c>
-      <c r="B68" t="n">
-        <v>20190510</v>
+      <c r="B68" s="2" t="n">
+        <v>43595</v>
       </c>
       <c r="C68" t="n">
         <v>112530</v>
@@ -3741,8 +3745,8 @@
       <c r="A69" s="1" t="n">
         <v>67</v>
       </c>
-      <c r="B69" t="n">
-        <v>20190510</v>
+      <c r="B69" s="2" t="n">
+        <v>43595</v>
       </c>
       <c r="C69" t="n">
         <v>112530</v>
@@ -3793,8 +3797,8 @@
       <c r="A70" s="1" t="n">
         <v>68</v>
       </c>
-      <c r="B70" t="n">
-        <v>20190510</v>
+      <c r="B70" s="2" t="n">
+        <v>43595</v>
       </c>
       <c r="C70" t="n">
         <v>112530</v>
@@ -3845,8 +3849,8 @@
       <c r="A71" s="1" t="n">
         <v>69</v>
       </c>
-      <c r="B71" t="n">
-        <v>20190510</v>
+      <c r="B71" s="2" t="n">
+        <v>43595</v>
       </c>
       <c r="C71" t="n">
         <v>112530</v>
@@ -3897,8 +3901,8 @@
       <c r="A72" s="1" t="n">
         <v>70</v>
       </c>
-      <c r="B72" t="n">
-        <v>20190510</v>
+      <c r="B72" s="2" t="n">
+        <v>43595</v>
       </c>
       <c r="C72" t="n">
         <v>112530</v>
@@ -3949,8 +3953,8 @@
       <c r="A73" s="1" t="n">
         <v>71</v>
       </c>
-      <c r="B73" t="n">
-        <v>20190510</v>
+      <c r="B73" s="2" t="n">
+        <v>43595</v>
       </c>
       <c r="C73" t="n">
         <v>112530</v>
@@ -4001,8 +4005,8 @@
       <c r="A74" s="1" t="n">
         <v>72</v>
       </c>
-      <c r="B74" t="n">
-        <v>20190510</v>
+      <c r="B74" s="2" t="n">
+        <v>43595</v>
       </c>
       <c r="C74" t="n">
         <v>112530</v>
@@ -4053,8 +4057,8 @@
       <c r="A75" s="1" t="n">
         <v>73</v>
       </c>
-      <c r="B75" t="n">
-        <v>20190510</v>
+      <c r="B75" s="2" t="n">
+        <v>43595</v>
       </c>
       <c r="C75" t="n">
         <v>112530</v>
@@ -4105,8 +4109,8 @@
       <c r="A76" s="1" t="n">
         <v>74</v>
       </c>
-      <c r="B76" t="n">
-        <v>20190510</v>
+      <c r="B76" s="2" t="n">
+        <v>43595</v>
       </c>
       <c r="C76" t="n">
         <v>112530</v>
@@ -4157,8 +4161,8 @@
       <c r="A77" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="B77" t="n">
-        <v>20190510</v>
+      <c r="B77" s="2" t="n">
+        <v>43595</v>
       </c>
       <c r="C77" t="n">
         <v>112530</v>
@@ -4209,8 +4213,8 @@
       <c r="A78" s="1" t="n">
         <v>76</v>
       </c>
-      <c r="B78" t="n">
-        <v>20190510</v>
+      <c r="B78" s="2" t="n">
+        <v>43595</v>
       </c>
       <c r="C78" t="n">
         <v>112530</v>
@@ -4261,8 +4265,8 @@
       <c r="A79" s="1" t="n">
         <v>77</v>
       </c>
-      <c r="B79" t="n">
-        <v>20190513</v>
+      <c r="B79" s="2" t="n">
+        <v>43598</v>
       </c>
       <c r="C79" t="n">
         <v>2059</v>
@@ -4305,8 +4309,8 @@
       <c r="A80" s="1" t="n">
         <v>78</v>
       </c>
-      <c r="B80" t="n">
-        <v>20190520</v>
+      <c r="B80" s="2" t="n">
+        <v>43605</v>
       </c>
       <c r="C80" t="n">
         <v>121617</v>
@@ -4357,8 +4361,8 @@
       <c r="A81" s="1" t="n">
         <v>79</v>
       </c>
-      <c r="B81" t="n">
-        <v>20190520</v>
+      <c r="B81" s="2" t="n">
+        <v>43605</v>
       </c>
       <c r="C81" t="n">
         <v>121617</v>
@@ -4409,8 +4413,8 @@
       <c r="A82" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="B82" t="n">
-        <v>20190523</v>
+      <c r="B82" s="2" t="n">
+        <v>43608</v>
       </c>
       <c r="C82" t="n">
         <v>115424</v>
@@ -4461,8 +4465,8 @@
       <c r="A83" s="1" t="n">
         <v>81</v>
       </c>
-      <c r="B83" t="n">
-        <v>20190523</v>
+      <c r="B83" s="2" t="n">
+        <v>43608</v>
       </c>
       <c r="C83" t="n">
         <v>125702</v>
@@ -4513,8 +4517,8 @@
       <c r="A84" s="1" t="n">
         <v>82</v>
       </c>
-      <c r="B84" t="n">
-        <v>20190523</v>
+      <c r="B84" s="2" t="n">
+        <v>43608</v>
       </c>
       <c r="C84" t="n">
         <v>133254</v>
@@ -4565,8 +4569,8 @@
       <c r="A85" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="B85" t="n">
-        <v>20190523</v>
+      <c r="B85" s="2" t="n">
+        <v>43608</v>
       </c>
       <c r="C85" t="n">
         <v>133254</v>
@@ -4617,8 +4621,8 @@
       <c r="A86" s="1" t="n">
         <v>84</v>
       </c>
-      <c r="B86" t="n">
-        <v>20190524</v>
+      <c r="B86" s="2" t="n">
+        <v>43609</v>
       </c>
       <c r="C86" t="n">
         <v>130851</v>
@@ -4669,8 +4673,8 @@
       <c r="A87" s="1" t="n">
         <v>85</v>
       </c>
-      <c r="B87" t="n">
-        <v>20190524</v>
+      <c r="B87" s="2" t="n">
+        <v>43609</v>
       </c>
       <c r="C87" t="n">
         <v>175616</v>
@@ -4721,8 +4725,8 @@
       <c r="A88" s="1" t="n">
         <v>86</v>
       </c>
-      <c r="B88" t="n">
-        <v>20190529</v>
+      <c r="B88" s="2" t="n">
+        <v>43614</v>
       </c>
       <c r="C88" t="n">
         <v>150647</v>
@@ -4773,8 +4777,8 @@
       <c r="A89" s="1" t="n">
         <v>87</v>
       </c>
-      <c r="B89" t="n">
-        <v>20190529</v>
+      <c r="B89" s="2" t="n">
+        <v>43614</v>
       </c>
       <c r="C89" t="n">
         <v>180101</v>
@@ -4825,8 +4829,8 @@
       <c r="A90" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="B90" t="n">
-        <v>20190529</v>
+      <c r="B90" s="2" t="n">
+        <v>43614</v>
       </c>
       <c r="C90" t="n">
         <v>180101</v>
@@ -4877,8 +4881,8 @@
       <c r="A91" s="1" t="n">
         <v>89</v>
       </c>
-      <c r="B91" t="n">
-        <v>20190529</v>
+      <c r="B91" s="2" t="n">
+        <v>43614</v>
       </c>
       <c r="C91" t="n">
         <v>180101</v>
@@ -4929,8 +4933,8 @@
       <c r="A92" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="B92" t="n">
-        <v>20190529</v>
+      <c r="B92" s="2" t="n">
+        <v>43614</v>
       </c>
       <c r="C92" t="n">
         <v>180101</v>
@@ -4981,8 +4985,8 @@
       <c r="A93" s="1" t="n">
         <v>91</v>
       </c>
-      <c r="B93" t="n">
-        <v>20190602</v>
+      <c r="B93" s="2" t="n">
+        <v>43618</v>
       </c>
       <c r="C93" t="n">
         <v>41107</v>
@@ -5025,8 +5029,8 @@
       <c r="A94" s="1" t="n">
         <v>92</v>
       </c>
-      <c r="B94" t="n">
-        <v>20190602</v>
+      <c r="B94" s="2" t="n">
+        <v>43618</v>
       </c>
       <c r="C94" t="n">
         <v>41107</v>
@@ -5069,8 +5073,8 @@
       <c r="A95" s="1" t="n">
         <v>93</v>
       </c>
-      <c r="B95" t="n">
-        <v>20190602</v>
+      <c r="B95" s="2" t="n">
+        <v>43618</v>
       </c>
       <c r="C95" t="n">
         <v>42253</v>
@@ -5113,8 +5117,8 @@
       <c r="A96" s="1" t="n">
         <v>94</v>
       </c>
-      <c r="B96" t="n">
-        <v>20190604</v>
+      <c r="B96" s="2" t="n">
+        <v>43620</v>
       </c>
       <c r="C96" t="n">
         <v>173547</v>
@@ -5161,8 +5165,8 @@
       <c r="A97" s="1" t="n">
         <v>95</v>
       </c>
-      <c r="B97" t="n">
-        <v>20190605</v>
+      <c r="B97" s="2" t="n">
+        <v>43621</v>
       </c>
       <c r="C97" t="n">
         <v>94231</v>
@@ -5205,8 +5209,8 @@
       <c r="A98" s="1" t="n">
         <v>96</v>
       </c>
-      <c r="B98" t="n">
-        <v>20190606</v>
+      <c r="B98" s="2" t="n">
+        <v>43622</v>
       </c>
       <c r="C98" t="n">
         <v>185503</v>
@@ -5257,8 +5261,8 @@
       <c r="A99" s="1" t="n">
         <v>97</v>
       </c>
-      <c r="B99" t="n">
-        <v>20190610</v>
+      <c r="B99" s="2" t="n">
+        <v>43626</v>
       </c>
       <c r="C99" t="n">
         <v>100009</v>
@@ -5309,8 +5313,8 @@
       <c r="A100" s="1" t="n">
         <v>98</v>
       </c>
-      <c r="B100" t="n">
-        <v>20190610</v>
+      <c r="B100" s="2" t="n">
+        <v>43626</v>
       </c>
       <c r="C100" t="n">
         <v>100009</v>
@@ -5361,8 +5365,8 @@
       <c r="A101" s="1" t="n">
         <v>99</v>
       </c>
-      <c r="B101" t="n">
-        <v>20190610</v>
+      <c r="B101" s="2" t="n">
+        <v>43626</v>
       </c>
       <c r="C101" t="n">
         <v>100009</v>
@@ -5413,8 +5417,8 @@
       <c r="A102" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="B102" t="n">
-        <v>20190610</v>
+      <c r="B102" s="2" t="n">
+        <v>43626</v>
       </c>
       <c r="C102" t="n">
         <v>100009</v>
@@ -5465,8 +5469,8 @@
       <c r="A103" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="B103" t="n">
-        <v>20190610</v>
+      <c r="B103" s="2" t="n">
+        <v>43626</v>
       </c>
       <c r="C103" t="n">
         <v>100010</v>
@@ -5517,8 +5521,8 @@
       <c r="A104" s="1" t="n">
         <v>102</v>
       </c>
-      <c r="B104" t="n">
-        <v>20190610</v>
+      <c r="B104" s="2" t="n">
+        <v>43626</v>
       </c>
       <c r="C104" t="n">
         <v>100010</v>
@@ -5569,8 +5573,8 @@
       <c r="A105" s="1" t="n">
         <v>103</v>
       </c>
-      <c r="B105" t="n">
-        <v>20190610</v>
+      <c r="B105" s="2" t="n">
+        <v>43626</v>
       </c>
       <c r="C105" t="n">
         <v>100010</v>
@@ -5621,8 +5625,8 @@
       <c r="A106" s="1" t="n">
         <v>104</v>
       </c>
-      <c r="B106" t="n">
-        <v>20190610</v>
+      <c r="B106" s="2" t="n">
+        <v>43626</v>
       </c>
       <c r="C106" t="n">
         <v>100010</v>
@@ -5673,8 +5677,8 @@
       <c r="A107" s="1" t="n">
         <v>105</v>
       </c>
-      <c r="B107" t="n">
-        <v>20190610</v>
+      <c r="B107" s="2" t="n">
+        <v>43626</v>
       </c>
       <c r="C107" t="n">
         <v>100010</v>
@@ -5725,8 +5729,8 @@
       <c r="A108" s="1" t="n">
         <v>106</v>
       </c>
-      <c r="B108" t="n">
-        <v>20190610</v>
+      <c r="B108" s="2" t="n">
+        <v>43626</v>
       </c>
       <c r="C108" t="n">
         <v>100010</v>
@@ -5777,8 +5781,8 @@
       <c r="A109" s="1" t="n">
         <v>107</v>
       </c>
-      <c r="B109" t="n">
-        <v>20190610</v>
+      <c r="B109" s="2" t="n">
+        <v>43626</v>
       </c>
       <c r="C109" t="n">
         <v>100010</v>
@@ -5829,8 +5833,8 @@
       <c r="A110" s="1" t="n">
         <v>108</v>
       </c>
-      <c r="B110" t="n">
-        <v>20190610</v>
+      <c r="B110" s="2" t="n">
+        <v>43626</v>
       </c>
       <c r="C110" t="n">
         <v>100010</v>
@@ -5881,8 +5885,8 @@
       <c r="A111" s="1" t="n">
         <v>109</v>
       </c>
-      <c r="B111" t="n">
-        <v>20190610</v>
+      <c r="B111" s="2" t="n">
+        <v>43626</v>
       </c>
       <c r="C111" t="n">
         <v>100010</v>
@@ -5933,8 +5937,8 @@
       <c r="A112" s="1" t="n">
         <v>110</v>
       </c>
-      <c r="B112" t="n">
-        <v>20190610</v>
+      <c r="B112" s="2" t="n">
+        <v>43626</v>
       </c>
       <c r="C112" t="n">
         <v>100010</v>
@@ -5985,8 +5989,8 @@
       <c r="A113" s="1" t="n">
         <v>111</v>
       </c>
-      <c r="B113" t="n">
-        <v>20190610</v>
+      <c r="B113" s="2" t="n">
+        <v>43626</v>
       </c>
       <c r="C113" t="n">
         <v>100010</v>
@@ -6037,8 +6041,8 @@
       <c r="A114" s="1" t="n">
         <v>112</v>
       </c>
-      <c r="B114" t="n">
-        <v>20190610</v>
+      <c r="B114" s="2" t="n">
+        <v>43626</v>
       </c>
       <c r="C114" t="n">
         <v>100011</v>
@@ -6089,8 +6093,8 @@
       <c r="A115" s="1" t="n">
         <v>113</v>
       </c>
-      <c r="B115" t="n">
-        <v>20190610</v>
+      <c r="B115" s="2" t="n">
+        <v>43626</v>
       </c>
       <c r="C115" t="n">
         <v>100011</v>
@@ -6141,8 +6145,8 @@
       <c r="A116" s="1" t="n">
         <v>114</v>
       </c>
-      <c r="B116" t="n">
-        <v>20190611</v>
+      <c r="B116" s="2" t="n">
+        <v>43627</v>
       </c>
       <c r="C116" t="n">
         <v>3456</v>
@@ -6185,8 +6189,8 @@
       <c r="A117" s="1" t="n">
         <v>115</v>
       </c>
-      <c r="B117" t="n">
-        <v>20190612</v>
+      <c r="B117" s="2" t="n">
+        <v>43628</v>
       </c>
       <c r="C117" t="n">
         <v>145226</v>
@@ -6237,8 +6241,8 @@
       <c r="A118" s="1" t="n">
         <v>116</v>
       </c>
-      <c r="B118" t="n">
-        <v>20190620</v>
+      <c r="B118" s="2" t="n">
+        <v>43636</v>
       </c>
       <c r="C118" t="n">
         <v>172638</v>
@@ -6289,8 +6293,8 @@
       <c r="A119" s="1" t="n">
         <v>117</v>
       </c>
-      <c r="B119" t="n">
-        <v>20190621</v>
+      <c r="B119" s="2" t="n">
+        <v>43637</v>
       </c>
       <c r="C119" t="n">
         <v>25111</v>
@@ -6333,8 +6337,8 @@
       <c r="A120" s="1" t="n">
         <v>118</v>
       </c>
-      <c r="B120" t="n">
-        <v>20190625</v>
+      <c r="B120" s="2" t="n">
+        <v>43641</v>
       </c>
       <c r="C120" t="n">
         <v>150417</v>
@@ -6385,8 +6389,8 @@
       <c r="A121" s="1" t="n">
         <v>119</v>
       </c>
-      <c r="B121" t="n">
-        <v>20190627</v>
+      <c r="B121" s="2" t="n">
+        <v>43643</v>
       </c>
       <c r="C121" t="n">
         <v>154408</v>
@@ -6433,8 +6437,8 @@
       <c r="A122" s="1" t="n">
         <v>120</v>
       </c>
-      <c r="B122" t="n">
-        <v>20190628</v>
+      <c r="B122" s="2" t="n">
+        <v>43644</v>
       </c>
       <c r="C122" t="n">
         <v>145345</v>
@@ -6485,8 +6489,8 @@
       <c r="A123" s="1" t="n">
         <v>121</v>
       </c>
-      <c r="B123" t="n">
-        <v>20190628</v>
+      <c r="B123" s="2" t="n">
+        <v>43644</v>
       </c>
       <c r="C123" t="n">
         <v>145345</v>
@@ -6537,8 +6541,8 @@
       <c r="A124" s="1" t="n">
         <v>122</v>
       </c>
-      <c r="B124" t="n">
-        <v>20190702</v>
+      <c r="B124" s="2" t="n">
+        <v>43648</v>
       </c>
       <c r="C124" t="n">
         <v>44550</v>
@@ -6581,8 +6585,8 @@
       <c r="A125" s="1" t="n">
         <v>123</v>
       </c>
-      <c r="B125" t="n">
-        <v>20190702</v>
+      <c r="B125" s="2" t="n">
+        <v>43648</v>
       </c>
       <c r="C125" t="n">
         <v>44801</v>
@@ -6625,8 +6629,8 @@
       <c r="A126" s="1" t="n">
         <v>124</v>
       </c>
-      <c r="B126" t="n">
-        <v>20190702</v>
+      <c r="B126" s="2" t="n">
+        <v>43648</v>
       </c>
       <c r="C126" t="n">
         <v>50046</v>
@@ -6669,8 +6673,8 @@
       <c r="A127" s="1" t="n">
         <v>125</v>
       </c>
-      <c r="B127" t="n">
-        <v>20190703</v>
+      <c r="B127" s="2" t="n">
+        <v>43649</v>
       </c>
       <c r="C127" t="n">
         <v>134123</v>
@@ -6717,8 +6721,8 @@
       <c r="A128" s="1" t="n">
         <v>126</v>
       </c>
-      <c r="B128" t="n">
-        <v>20190708</v>
+      <c r="B128" s="2" t="n">
+        <v>43654</v>
       </c>
       <c r="C128" t="n">
         <v>101616</v>
@@ -6769,8 +6773,8 @@
       <c r="A129" s="1" t="n">
         <v>127</v>
       </c>
-      <c r="B129" t="n">
-        <v>20190708</v>
+      <c r="B129" s="2" t="n">
+        <v>43654</v>
       </c>
       <c r="C129" t="n">
         <v>150849</v>
@@ -6817,8 +6821,8 @@
       <c r="A130" s="1" t="n">
         <v>128</v>
       </c>
-      <c r="B130" t="n">
-        <v>20190708</v>
+      <c r="B130" s="2" t="n">
+        <v>43654</v>
       </c>
       <c r="C130" t="n">
         <v>151747</v>
@@ -6865,8 +6869,8 @@
       <c r="A131" s="1" t="n">
         <v>129</v>
       </c>
-      <c r="B131" t="n">
-        <v>20190708</v>
+      <c r="B131" s="2" t="n">
+        <v>43654</v>
       </c>
       <c r="C131" t="n">
         <v>152134</v>
@@ -6909,8 +6913,8 @@
       <c r="A132" s="1" t="n">
         <v>130</v>
       </c>
-      <c r="B132" t="n">
-        <v>20190710</v>
+      <c r="B132" s="2" t="n">
+        <v>43656</v>
       </c>
       <c r="C132" t="n">
         <v>114900</v>
@@ -6961,8 +6965,8 @@
       <c r="A133" s="1" t="n">
         <v>131</v>
       </c>
-      <c r="B133" t="n">
-        <v>20190710</v>
+      <c r="B133" s="2" t="n">
+        <v>43656</v>
       </c>
       <c r="C133" t="n">
         <v>114900</v>
@@ -7013,8 +7017,8 @@
       <c r="A134" s="1" t="n">
         <v>132</v>
       </c>
-      <c r="B134" t="n">
-        <v>20190710</v>
+      <c r="B134" s="2" t="n">
+        <v>43656</v>
       </c>
       <c r="C134" t="n">
         <v>114900</v>
@@ -7065,8 +7069,8 @@
       <c r="A135" s="1" t="n">
         <v>133</v>
       </c>
-      <c r="B135" t="n">
-        <v>20190710</v>
+      <c r="B135" s="2" t="n">
+        <v>43656</v>
       </c>
       <c r="C135" t="n">
         <v>114900</v>
@@ -7117,8 +7121,8 @@
       <c r="A136" s="1" t="n">
         <v>134</v>
       </c>
-      <c r="B136" t="n">
-        <v>20190710</v>
+      <c r="B136" s="2" t="n">
+        <v>43656</v>
       </c>
       <c r="C136" t="n">
         <v>114900</v>
@@ -7169,8 +7173,8 @@
       <c r="A137" s="1" t="n">
         <v>135</v>
       </c>
-      <c r="B137" t="n">
-        <v>20190710</v>
+      <c r="B137" s="2" t="n">
+        <v>43656</v>
       </c>
       <c r="C137" t="n">
         <v>114900</v>
@@ -7221,8 +7225,8 @@
       <c r="A138" s="1" t="n">
         <v>136</v>
       </c>
-      <c r="B138" t="n">
-        <v>20190710</v>
+      <c r="B138" s="2" t="n">
+        <v>43656</v>
       </c>
       <c r="C138" t="n">
         <v>114900</v>
@@ -7273,8 +7277,8 @@
       <c r="A139" s="1" t="n">
         <v>137</v>
       </c>
-      <c r="B139" t="n">
-        <v>20190710</v>
+      <c r="B139" s="2" t="n">
+        <v>43656</v>
       </c>
       <c r="C139" t="n">
         <v>114900</v>
@@ -7325,8 +7329,8 @@
       <c r="A140" s="1" t="n">
         <v>138</v>
       </c>
-      <c r="B140" t="n">
-        <v>20190710</v>
+      <c r="B140" s="2" t="n">
+        <v>43656</v>
       </c>
       <c r="C140" t="n">
         <v>114900</v>
@@ -7377,8 +7381,8 @@
       <c r="A141" s="1" t="n">
         <v>139</v>
       </c>
-      <c r="B141" t="n">
-        <v>20190710</v>
+      <c r="B141" s="2" t="n">
+        <v>43656</v>
       </c>
       <c r="C141" t="n">
         <v>114900</v>
@@ -7429,8 +7433,8 @@
       <c r="A142" s="1" t="n">
         <v>140</v>
       </c>
-      <c r="B142" t="n">
-        <v>20190710</v>
+      <c r="B142" s="2" t="n">
+        <v>43656</v>
       </c>
       <c r="C142" t="n">
         <v>114900</v>
@@ -7481,8 +7485,8 @@
       <c r="A143" s="1" t="n">
         <v>141</v>
       </c>
-      <c r="B143" t="n">
-        <v>20190710</v>
+      <c r="B143" s="2" t="n">
+        <v>43656</v>
       </c>
       <c r="C143" t="n">
         <v>114900</v>
@@ -7533,8 +7537,8 @@
       <c r="A144" s="1" t="n">
         <v>142</v>
       </c>
-      <c r="B144" t="n">
-        <v>20190711</v>
+      <c r="B144" s="2" t="n">
+        <v>43657</v>
       </c>
       <c r="C144" t="n">
         <v>3618</v>
@@ -7577,8 +7581,8 @@
       <c r="A145" s="1" t="n">
         <v>143</v>
       </c>
-      <c r="B145" t="n">
-        <v>20190712</v>
+      <c r="B145" s="2" t="n">
+        <v>43658</v>
       </c>
       <c r="C145" t="n">
         <v>175932</v>
@@ -7629,8 +7633,8 @@
       <c r="A146" s="1" t="n">
         <v>144</v>
       </c>
-      <c r="B146" t="n">
-        <v>20190712</v>
+      <c r="B146" s="2" t="n">
+        <v>43658</v>
       </c>
       <c r="C146" t="n">
         <v>175932</v>
@@ -7681,8 +7685,8 @@
       <c r="A147" s="1" t="n">
         <v>145</v>
       </c>
-      <c r="B147" t="n">
-        <v>20190712</v>
+      <c r="B147" s="2" t="n">
+        <v>43658</v>
       </c>
       <c r="C147" t="n">
         <v>175932</v>
@@ -7733,8 +7737,8 @@
       <c r="A148" s="1" t="n">
         <v>146</v>
       </c>
-      <c r="B148" t="n">
-        <v>20190717</v>
+      <c r="B148" s="2" t="n">
+        <v>43663</v>
       </c>
       <c r="C148" t="n">
         <v>171533</v>
@@ -7785,8 +7789,8 @@
       <c r="A149" s="1" t="n">
         <v>147</v>
       </c>
-      <c r="B149" t="n">
-        <v>20190725</v>
+      <c r="B149" s="2" t="n">
+        <v>43671</v>
       </c>
       <c r="C149" t="n">
         <v>174522</v>
@@ -7833,8 +7837,8 @@
       <c r="A150" s="1" t="n">
         <v>148</v>
       </c>
-      <c r="B150" t="n">
-        <v>20190731</v>
+      <c r="B150" s="2" t="n">
+        <v>43677</v>
       </c>
       <c r="C150" t="n">
         <v>105338</v>
@@ -7885,8 +7889,8 @@
       <c r="A151" s="1" t="n">
         <v>149</v>
       </c>
-      <c r="B151" t="n">
-        <v>20190731</v>
+      <c r="B151" s="2" t="n">
+        <v>43677</v>
       </c>
       <c r="C151" t="n">
         <v>154251</v>
@@ -7937,8 +7941,8 @@
       <c r="A152" s="1" t="n">
         <v>150</v>
       </c>
-      <c r="B152" t="n">
-        <v>20190801</v>
+      <c r="B152" s="2" t="n">
+        <v>43678</v>
       </c>
       <c r="C152" t="n">
         <v>151257</v>
@@ -7985,8 +7989,8 @@
       <c r="A153" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="B153" t="n">
-        <v>20190801</v>
+      <c r="B153" s="2" t="n">
+        <v>43678</v>
       </c>
       <c r="C153" t="n">
         <v>173309</v>
@@ -8037,8 +8041,8 @@
       <c r="A154" s="1" t="n">
         <v>152</v>
       </c>
-      <c r="B154" t="n">
-        <v>20190802</v>
+      <c r="B154" s="2" t="n">
+        <v>43679</v>
       </c>
       <c r="C154" t="n">
         <v>40719</v>
@@ -8081,8 +8085,8 @@
       <c r="A155" s="1" t="n">
         <v>153</v>
       </c>
-      <c r="B155" t="n">
-        <v>20190802</v>
+      <c r="B155" s="2" t="n">
+        <v>43679</v>
       </c>
       <c r="C155" t="n">
         <v>40719</v>
@@ -8125,8 +8129,8 @@
       <c r="A156" s="1" t="n">
         <v>154</v>
       </c>
-      <c r="B156" t="n">
-        <v>20190802</v>
+      <c r="B156" s="2" t="n">
+        <v>43679</v>
       </c>
       <c r="C156" t="n">
         <v>42848</v>
@@ -8169,8 +8173,8 @@
       <c r="A157" s="1" t="n">
         <v>155</v>
       </c>
-      <c r="B157" t="n">
-        <v>20190806</v>
+      <c r="B157" s="2" t="n">
+        <v>43683</v>
       </c>
       <c r="C157" t="n">
         <v>102821</v>
@@ -8217,8 +8221,8 @@
       <c r="A158" s="1" t="n">
         <v>156</v>
       </c>
-      <c r="B158" t="n">
-        <v>20190806</v>
+      <c r="B158" s="2" t="n">
+        <v>43683</v>
       </c>
       <c r="C158" t="n">
         <v>160946</v>
@@ -8269,8 +8273,8 @@
       <c r="A159" s="1" t="n">
         <v>157</v>
       </c>
-      <c r="B159" t="n">
-        <v>20190809</v>
+      <c r="B159" s="2" t="n">
+        <v>43686</v>
       </c>
       <c r="C159" t="n">
         <v>100644</v>
@@ -8317,8 +8321,8 @@
       <c r="A160" s="1" t="n">
         <v>158</v>
       </c>
-      <c r="B160" t="n">
-        <v>20190809</v>
+      <c r="B160" s="2" t="n">
+        <v>43686</v>
       </c>
       <c r="C160" t="n">
         <v>110847</v>
@@ -8369,8 +8373,8 @@
       <c r="A161" s="1" t="n">
         <v>159</v>
       </c>
-      <c r="B161" t="n">
-        <v>20190809</v>
+      <c r="B161" s="2" t="n">
+        <v>43686</v>
       </c>
       <c r="C161" t="n">
         <v>140516</v>
@@ -8421,8 +8425,8 @@
       <c r="A162" s="1" t="n">
         <v>160</v>
       </c>
-      <c r="B162" t="n">
-        <v>20190809</v>
+      <c r="B162" s="2" t="n">
+        <v>43686</v>
       </c>
       <c r="C162" t="n">
         <v>140516</v>
@@ -8473,8 +8477,8 @@
       <c r="A163" s="1" t="n">
         <v>161</v>
       </c>
-      <c r="B163" t="n">
-        <v>20190809</v>
+      <c r="B163" s="2" t="n">
+        <v>43686</v>
       </c>
       <c r="C163" t="n">
         <v>140516</v>
@@ -8525,8 +8529,8 @@
       <c r="A164" s="1" t="n">
         <v>162</v>
       </c>
-      <c r="B164" t="n">
-        <v>20190809</v>
+      <c r="B164" s="2" t="n">
+        <v>43686</v>
       </c>
       <c r="C164" t="n">
         <v>140516</v>
@@ -8577,8 +8581,8 @@
       <c r="A165" s="1" t="n">
         <v>163</v>
       </c>
-      <c r="B165" t="n">
-        <v>20190809</v>
+      <c r="B165" s="2" t="n">
+        <v>43686</v>
       </c>
       <c r="C165" t="n">
         <v>140516</v>
@@ -8629,8 +8633,8 @@
       <c r="A166" s="1" t="n">
         <v>164</v>
       </c>
-      <c r="B166" t="n">
-        <v>20190809</v>
+      <c r="B166" s="2" t="n">
+        <v>43686</v>
       </c>
       <c r="C166" t="n">
         <v>140522</v>
@@ -8673,8 +8677,8 @@
       <c r="A167" s="1" t="n">
         <v>165</v>
       </c>
-      <c r="B167" t="n">
-        <v>20190809</v>
+      <c r="B167" s="2" t="n">
+        <v>43686</v>
       </c>
       <c r="C167" t="n">
         <v>140528</v>
@@ -8717,8 +8721,8 @@
       <c r="A168" s="1" t="n">
         <v>166</v>
       </c>
-      <c r="B168" t="n">
-        <v>20190809</v>
+      <c r="B168" s="2" t="n">
+        <v>43686</v>
       </c>
       <c r="C168" t="n">
         <v>143912</v>
@@ -8761,8 +8765,8 @@
       <c r="A169" s="1" t="n">
         <v>167</v>
       </c>
-      <c r="B169" t="n">
-        <v>20190812</v>
+      <c r="B169" s="2" t="n">
+        <v>43689</v>
       </c>
       <c r="C169" t="n">
         <v>100818</v>
@@ -8809,8 +8813,8 @@
       <c r="A170" s="1" t="n">
         <v>168</v>
       </c>
-      <c r="B170" t="n">
-        <v>20190813</v>
+      <c r="B170" s="2" t="n">
+        <v>43690</v>
       </c>
       <c r="C170" t="n">
         <v>921</v>
@@ -8853,8 +8857,8 @@
       <c r="A171" s="1" t="n">
         <v>169</v>
       </c>
-      <c r="B171" t="n">
-        <v>20190814</v>
+      <c r="B171" s="2" t="n">
+        <v>43691</v>
       </c>
       <c r="C171" t="n">
         <v>172724</v>
@@ -8905,8 +8909,8 @@
       <c r="A172" s="1" t="n">
         <v>170</v>
       </c>
-      <c r="B172" t="n">
-        <v>20190819</v>
+      <c r="B172" s="2" t="n">
+        <v>43696</v>
       </c>
       <c r="C172" t="n">
         <v>154900</v>
@@ -8953,8 +8957,8 @@
       <c r="A173" s="1" t="n">
         <v>171</v>
       </c>
-      <c r="B173" t="n">
-        <v>20190820</v>
+      <c r="B173" s="2" t="n">
+        <v>43697</v>
       </c>
       <c r="C173" t="n">
         <v>155153</v>
@@ -9005,8 +9009,8 @@
       <c r="A174" s="1" t="n">
         <v>172</v>
       </c>
-      <c r="B174" t="n">
-        <v>20190830</v>
+      <c r="B174" s="2" t="n">
+        <v>43707</v>
       </c>
       <c r="C174" t="n">
         <v>102306</v>
@@ -9053,8 +9057,8 @@
       <c r="A175" s="1" t="n">
         <v>173</v>
       </c>
-      <c r="B175" t="n">
-        <v>20190830</v>
+      <c r="B175" s="2" t="n">
+        <v>43707</v>
       </c>
       <c r="C175" t="n">
         <v>120010</v>
@@ -9105,8 +9109,8 @@
       <c r="A176" s="1" t="n">
         <v>174</v>
       </c>
-      <c r="B176" t="n">
-        <v>20190830</v>
+      <c r="B176" s="2" t="n">
+        <v>43707</v>
       </c>
       <c r="C176" t="n">
         <v>120010</v>
@@ -9157,8 +9161,8 @@
       <c r="A177" s="1" t="n">
         <v>175</v>
       </c>
-      <c r="B177" t="n">
-        <v>20190902</v>
+      <c r="B177" s="2" t="n">
+        <v>43710</v>
       </c>
       <c r="C177" t="n">
         <v>35741</v>
@@ -9201,8 +9205,8 @@
       <c r="A178" s="1" t="n">
         <v>176</v>
       </c>
-      <c r="B178" t="n">
-        <v>20190902</v>
+      <c r="B178" s="2" t="n">
+        <v>43710</v>
       </c>
       <c r="C178" t="n">
         <v>41501</v>
@@ -9245,8 +9249,8 @@
       <c r="A179" s="1" t="n">
         <v>177</v>
       </c>
-      <c r="B179" t="n">
-        <v>20190902</v>
+      <c r="B179" s="2" t="n">
+        <v>43710</v>
       </c>
       <c r="C179" t="n">
         <v>42410</v>
@@ -9289,8 +9293,8 @@
       <c r="A180" s="1" t="n">
         <v>178</v>
       </c>
-      <c r="B180" t="n">
-        <v>20190909</v>
+      <c r="B180" s="2" t="n">
+        <v>43717</v>
       </c>
       <c r="C180" t="n">
         <v>101547</v>
@@ -9337,8 +9341,8 @@
       <c r="A181" s="1" t="n">
         <v>179</v>
       </c>
-      <c r="B181" t="n">
-        <v>20190909</v>
+      <c r="B181" s="2" t="n">
+        <v>43717</v>
       </c>
       <c r="C181" t="n">
         <v>114533</v>
@@ -9389,8 +9393,8 @@
       <c r="A182" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="B182" t="n">
-        <v>20190910</v>
+      <c r="B182" s="2" t="n">
+        <v>43718</v>
       </c>
       <c r="C182" t="n">
         <v>100037</v>
@@ -9437,8 +9441,8 @@
       <c r="A183" s="1" t="n">
         <v>181</v>
       </c>
-      <c r="B183" t="n">
-        <v>20190910</v>
+      <c r="B183" s="2" t="n">
+        <v>43718</v>
       </c>
       <c r="C183" t="n">
         <v>110647</v>
@@ -9481,8 +9485,8 @@
       <c r="A184" s="1" t="n">
         <v>182</v>
       </c>
-      <c r="B184" t="n">
-        <v>20190910</v>
+      <c r="B184" s="2" t="n">
+        <v>43718</v>
       </c>
       <c r="C184" t="n">
         <v>110652</v>
@@ -9525,8 +9529,8 @@
       <c r="A185" s="1" t="n">
         <v>183</v>
       </c>
-      <c r="B185" t="n">
-        <v>20190910</v>
+      <c r="B185" s="2" t="n">
+        <v>43718</v>
       </c>
       <c r="C185" t="n">
         <v>110743</v>
@@ -9577,8 +9581,8 @@
       <c r="A186" s="1" t="n">
         <v>184</v>
       </c>
-      <c r="B186" t="n">
-        <v>20190910</v>
+      <c r="B186" s="2" t="n">
+        <v>43718</v>
       </c>
       <c r="C186" t="n">
         <v>110743</v>
@@ -9629,8 +9633,8 @@
       <c r="A187" s="1" t="n">
         <v>185</v>
       </c>
-      <c r="B187" t="n">
-        <v>20190910</v>
+      <c r="B187" s="2" t="n">
+        <v>43718</v>
       </c>
       <c r="C187" t="n">
         <v>110743</v>
@@ -9681,8 +9685,8 @@
       <c r="A188" s="1" t="n">
         <v>186</v>
       </c>
-      <c r="B188" t="n">
-        <v>20190910</v>
+      <c r="B188" s="2" t="n">
+        <v>43718</v>
       </c>
       <c r="C188" t="n">
         <v>110743</v>
@@ -9733,8 +9737,8 @@
       <c r="A189" s="1" t="n">
         <v>187</v>
       </c>
-      <c r="B189" t="n">
-        <v>20190910</v>
+      <c r="B189" s="2" t="n">
+        <v>43718</v>
       </c>
       <c r="C189" t="n">
         <v>110744</v>
@@ -9785,8 +9789,8 @@
       <c r="A190" s="1" t="n">
         <v>188</v>
       </c>
-      <c r="B190" t="n">
-        <v>20190910</v>
+      <c r="B190" s="2" t="n">
+        <v>43718</v>
       </c>
       <c r="C190" t="n">
         <v>110744</v>
@@ -9837,8 +9841,8 @@
       <c r="A191" s="1" t="n">
         <v>189</v>
       </c>
-      <c r="B191" t="n">
-        <v>20190910</v>
+      <c r="B191" s="2" t="n">
+        <v>43718</v>
       </c>
       <c r="C191" t="n">
         <v>110744</v>
@@ -9889,8 +9893,8 @@
       <c r="A192" s="1" t="n">
         <v>190</v>
       </c>
-      <c r="B192" t="n">
-        <v>20190910</v>
+      <c r="B192" s="2" t="n">
+        <v>43718</v>
       </c>
       <c r="C192" t="n">
         <v>110744</v>
@@ -9941,8 +9945,8 @@
       <c r="A193" s="1" t="n">
         <v>191</v>
       </c>
-      <c r="B193" t="n">
-        <v>20190910</v>
+      <c r="B193" s="2" t="n">
+        <v>43718</v>
       </c>
       <c r="C193" t="n">
         <v>115951</v>
@@ -9985,8 +9989,8 @@
       <c r="A194" s="1" t="n">
         <v>192</v>
       </c>
-      <c r="B194" t="n">
-        <v>20190910</v>
+      <c r="B194" s="2" t="n">
+        <v>43718</v>
       </c>
       <c r="C194" t="n">
         <v>152133</v>
@@ -10033,8 +10037,8 @@
       <c r="A195" s="1" t="n">
         <v>193</v>
       </c>
-      <c r="B195" t="n">
-        <v>20190911</v>
+      <c r="B195" s="2" t="n">
+        <v>43719</v>
       </c>
       <c r="C195" t="n">
         <v>10223</v>
@@ -10077,8 +10081,8 @@
       <c r="A196" s="1" t="n">
         <v>194</v>
       </c>
-      <c r="B196" t="n">
-        <v>20190911</v>
+      <c r="B196" s="2" t="n">
+        <v>43719</v>
       </c>
       <c r="C196" t="n">
         <v>102139</v>
@@ -10125,8 +10129,8 @@
       <c r="A197" s="1" t="n">
         <v>195</v>
       </c>
-      <c r="B197" t="n">
-        <v>20190911</v>
+      <c r="B197" s="2" t="n">
+        <v>43719</v>
       </c>
       <c r="C197" t="n">
         <v>102807</v>
@@ -10177,8 +10181,8 @@
       <c r="A198" s="1" t="n">
         <v>196</v>
       </c>
-      <c r="B198" t="n">
-        <v>20190921</v>
+      <c r="B198" s="2" t="n">
+        <v>43729</v>
       </c>
       <c r="C198" t="n">
         <v>24243</v>
@@ -10221,8 +10225,8 @@
       <c r="A199" s="1" t="n">
         <v>197</v>
       </c>
-      <c r="B199" t="n">
-        <v>20190929</v>
+      <c r="B199" s="2" t="n">
+        <v>43737</v>
       </c>
       <c r="C199" t="n">
         <v>94231</v>
@@ -10269,8 +10273,8 @@
       <c r="A200" s="1" t="n">
         <v>198</v>
       </c>
-      <c r="B200" t="n">
-        <v>20190929</v>
+      <c r="B200" s="2" t="n">
+        <v>43737</v>
       </c>
       <c r="C200" t="n">
         <v>120435</v>
@@ -10321,8 +10325,8 @@
       <c r="A201" s="1" t="n">
         <v>199</v>
       </c>
-      <c r="B201" t="n">
-        <v>20190929</v>
+      <c r="B201" s="2" t="n">
+        <v>43737</v>
       </c>
       <c r="C201" t="n">
         <v>120435</v>
@@ -10373,8 +10377,8 @@
       <c r="A202" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="B202" t="n">
-        <v>20191002</v>
+      <c r="B202" s="2" t="n">
+        <v>43740</v>
       </c>
       <c r="C202" t="n">
         <v>40139</v>
@@ -10417,8 +10421,8 @@
       <c r="A203" s="1" t="n">
         <v>201</v>
       </c>
-      <c r="B203" t="n">
-        <v>20191002</v>
+      <c r="B203" s="2" t="n">
+        <v>43740</v>
       </c>
       <c r="C203" t="n">
         <v>40309</v>
@@ -10461,8 +10465,8 @@
       <c r="A204" s="1" t="n">
         <v>202</v>
       </c>
-      <c r="B204" t="n">
-        <v>20191002</v>
+      <c r="B204" s="2" t="n">
+        <v>43740</v>
       </c>
       <c r="C204" t="n">
         <v>44421</v>
@@ -10505,8 +10509,8 @@
       <c r="A205" s="1" t="n">
         <v>203</v>
       </c>
-      <c r="B205" t="n">
-        <v>20191010</v>
+      <c r="B205" s="2" t="n">
+        <v>43748</v>
       </c>
       <c r="C205" t="n">
         <v>91135</v>
@@ -10557,8 +10561,8 @@
       <c r="A206" s="1" t="n">
         <v>204</v>
       </c>
-      <c r="B206" t="n">
-        <v>20191010</v>
+      <c r="B206" s="2" t="n">
+        <v>43748</v>
       </c>
       <c r="C206" t="n">
         <v>115902</v>
@@ -10609,8 +10613,8 @@
       <c r="A207" s="1" t="n">
         <v>205</v>
       </c>
-      <c r="B207" t="n">
-        <v>20191010</v>
+      <c r="B207" s="2" t="n">
+        <v>43748</v>
       </c>
       <c r="C207" t="n">
         <v>143231</v>
@@ -10653,8 +10657,8 @@
       <c r="A208" s="1" t="n">
         <v>206</v>
       </c>
-      <c r="B208" t="n">
-        <v>20191010</v>
+      <c r="B208" s="2" t="n">
+        <v>43748</v>
       </c>
       <c r="C208" t="n">
         <v>154308</v>
@@ -10701,8 +10705,8 @@
       <c r="A209" s="1" t="n">
         <v>207</v>
       </c>
-      <c r="B209" t="n">
-        <v>20191010</v>
+      <c r="B209" s="2" t="n">
+        <v>43748</v>
       </c>
       <c r="C209" t="n">
         <v>234934</v>
@@ -10753,8 +10757,8 @@
       <c r="A210" s="1" t="n">
         <v>208</v>
       </c>
-      <c r="B210" t="n">
-        <v>20191010</v>
+      <c r="B210" s="2" t="n">
+        <v>43748</v>
       </c>
       <c r="C210" t="n">
         <v>234934</v>
@@ -10805,8 +10809,8 @@
       <c r="A211" s="1" t="n">
         <v>209</v>
       </c>
-      <c r="B211" t="n">
-        <v>20191010</v>
+      <c r="B211" s="2" t="n">
+        <v>43748</v>
       </c>
       <c r="C211" t="n">
         <v>234934</v>
@@ -10857,8 +10861,8 @@
       <c r="A212" s="1" t="n">
         <v>210</v>
       </c>
-      <c r="B212" t="n">
-        <v>20191010</v>
+      <c r="B212" s="2" t="n">
+        <v>43748</v>
       </c>
       <c r="C212" t="n">
         <v>234959</v>
@@ -10901,8 +10905,8 @@
       <c r="A213" s="1" t="n">
         <v>211</v>
       </c>
-      <c r="B213" t="n">
-        <v>20191010</v>
+      <c r="B213" s="2" t="n">
+        <v>43748</v>
       </c>
       <c r="C213" t="n">
         <v>235013</v>
@@ -10945,8 +10949,8 @@
       <c r="A214" s="1" t="n">
         <v>212</v>
       </c>
-      <c r="B214" t="n">
-        <v>20191011</v>
+      <c r="B214" s="2" t="n">
+        <v>43749</v>
       </c>
       <c r="C214" t="n">
         <v>4719</v>
@@ -10989,8 +10993,8 @@
       <c r="A215" s="1" t="n">
         <v>213</v>
       </c>
-      <c r="B215" t="n">
-        <v>20191012</v>
+      <c r="B215" s="2" t="n">
+        <v>43750</v>
       </c>
       <c r="C215" t="n">
         <v>100856</v>
@@ -11037,8 +11041,8 @@
       <c r="A216" s="1" t="n">
         <v>214</v>
       </c>
-      <c r="B216" t="n">
-        <v>20191018</v>
+      <c r="B216" s="2" t="n">
+        <v>43756</v>
       </c>
       <c r="C216" t="n">
         <v>121851</v>
@@ -11085,8 +11089,8 @@
       <c r="A217" s="1" t="n">
         <v>215</v>
       </c>
-      <c r="B217" t="n">
-        <v>20191018</v>
+      <c r="B217" s="2" t="n">
+        <v>43756</v>
       </c>
       <c r="C217" t="n">
         <v>122900</v>
@@ -11137,8 +11141,8 @@
       <c r="A218" s="1" t="n">
         <v>216</v>
       </c>
-      <c r="B218" t="n">
-        <v>20191018</v>
+      <c r="B218" s="2" t="n">
+        <v>43756</v>
       </c>
       <c r="C218" t="n">
         <v>182905</v>
@@ -11189,8 +11193,8 @@
       <c r="A219" s="1" t="n">
         <v>217</v>
       </c>
-      <c r="B219" t="n">
-        <v>20191018</v>
+      <c r="B219" s="2" t="n">
+        <v>43756</v>
       </c>
       <c r="C219" t="n">
         <v>182905</v>
@@ -11241,8 +11245,8 @@
       <c r="A220" s="1" t="n">
         <v>218</v>
       </c>
-      <c r="B220" t="n">
-        <v>20191024</v>
+      <c r="B220" s="2" t="n">
+        <v>43762</v>
       </c>
       <c r="C220" t="n">
         <v>113913</v>
@@ -11293,8 +11297,8 @@
       <c r="A221" s="1" t="n">
         <v>219</v>
       </c>
-      <c r="B221" t="n">
-        <v>20191030</v>
+      <c r="B221" s="2" t="n">
+        <v>43768</v>
       </c>
       <c r="C221" t="n">
         <v>141336</v>
@@ -11345,8 +11349,8 @@
       <c r="A222" s="1" t="n">
         <v>220</v>
       </c>
-      <c r="B222" t="n">
-        <v>20191030</v>
+      <c r="B222" s="2" t="n">
+        <v>43768</v>
       </c>
       <c r="C222" t="n">
         <v>143400</v>
@@ -11397,8 +11401,8 @@
       <c r="A223" s="1" t="n">
         <v>221</v>
       </c>
-      <c r="B223" t="n">
-        <v>20191030</v>
+      <c r="B223" s="2" t="n">
+        <v>43768</v>
       </c>
       <c r="C223" t="n">
         <v>143400</v>
@@ -11449,8 +11453,8 @@
       <c r="A224" s="1" t="n">
         <v>222</v>
       </c>
-      <c r="B224" t="n">
-        <v>20191030</v>
+      <c r="B224" s="2" t="n">
+        <v>43768</v>
       </c>
       <c r="C224" t="n">
         <v>183729</v>
@@ -11501,8 +11505,8 @@
       <c r="A225" s="1" t="n">
         <v>223</v>
       </c>
-      <c r="B225" t="n">
-        <v>20191030</v>
+      <c r="B225" s="2" t="n">
+        <v>43768</v>
       </c>
       <c r="C225" t="n">
         <v>192000</v>
@@ -11553,8 +11557,8 @@
       <c r="A226" s="1" t="n">
         <v>224</v>
       </c>
-      <c r="B226" t="n">
-        <v>20191101</v>
+      <c r="B226" s="2" t="n">
+        <v>43770</v>
       </c>
       <c r="C226" t="n">
         <v>114745</v>
@@ -11605,8 +11609,8 @@
       <c r="A227" s="1" t="n">
         <v>225</v>
       </c>
-      <c r="B227" t="n">
-        <v>20191102</v>
+      <c r="B227" s="2" t="n">
+        <v>43771</v>
       </c>
       <c r="C227" t="n">
         <v>41546</v>
@@ -11649,8 +11653,8 @@
       <c r="A228" s="1" t="n">
         <v>226</v>
       </c>
-      <c r="B228" t="n">
-        <v>20191102</v>
+      <c r="B228" s="2" t="n">
+        <v>43771</v>
       </c>
       <c r="C228" t="n">
         <v>41724</v>
@@ -11693,8 +11697,8 @@
       <c r="A229" s="1" t="n">
         <v>227</v>
       </c>
-      <c r="B229" t="n">
-        <v>20191102</v>
+      <c r="B229" s="2" t="n">
+        <v>43771</v>
       </c>
       <c r="C229" t="n">
         <v>44649</v>
@@ -11737,8 +11741,8 @@
       <c r="A230" s="1" t="n">
         <v>228</v>
       </c>
-      <c r="B230" t="n">
-        <v>20191103</v>
+      <c r="B230" s="2" t="n">
+        <v>43772</v>
       </c>
       <c r="C230" t="n">
         <v>134706</v>
@@ -11781,8 +11785,8 @@
       <c r="A231" s="1" t="n">
         <v>229</v>
       </c>
-      <c r="B231" t="n">
-        <v>20191106</v>
+      <c r="B231" s="2" t="n">
+        <v>43775</v>
       </c>
       <c r="C231" t="n">
         <v>165720</v>
@@ -11833,8 +11837,8 @@
       <c r="A232" s="1" t="n">
         <v>230</v>
       </c>
-      <c r="B232" t="n">
-        <v>20191107</v>
+      <c r="B232" s="2" t="n">
+        <v>43776</v>
       </c>
       <c r="C232" t="n">
         <v>152904</v>
@@ -11881,8 +11885,8 @@
       <c r="A233" s="1" t="n">
         <v>231</v>
       </c>
-      <c r="B233" t="n">
-        <v>20191108</v>
+      <c r="B233" s="2" t="n">
+        <v>43777</v>
       </c>
       <c r="C233" t="n">
         <v>111231</v>
@@ -11933,8 +11937,8 @@
       <c r="A234" s="1" t="n">
         <v>232</v>
       </c>
-      <c r="B234" t="n">
-        <v>20191108</v>
+      <c r="B234" s="2" t="n">
+        <v>43777</v>
       </c>
       <c r="C234" t="n">
         <v>121430</v>
@@ -11985,8 +11989,8 @@
       <c r="A235" s="1" t="n">
         <v>233</v>
       </c>
-      <c r="B235" t="n">
-        <v>20191108</v>
+      <c r="B235" s="2" t="n">
+        <v>43777</v>
       </c>
       <c r="C235" t="n">
         <v>121512</v>
@@ -12029,8 +12033,8 @@
       <c r="A236" s="1" t="n">
         <v>234</v>
       </c>
-      <c r="B236" t="n">
-        <v>20191108</v>
+      <c r="B236" s="2" t="n">
+        <v>43777</v>
       </c>
       <c r="C236" t="n">
         <v>121519</v>
@@ -12073,8 +12077,8 @@
       <c r="A237" s="1" t="n">
         <v>235</v>
       </c>
-      <c r="B237" t="n">
-        <v>20191111</v>
+      <c r="B237" s="2" t="n">
+        <v>43780</v>
       </c>
       <c r="C237" t="n">
         <v>113432</v>
@@ -12117,8 +12121,8 @@
       <c r="A238" s="1" t="n">
         <v>236</v>
       </c>
-      <c r="B238" t="n">
-        <v>20191111</v>
+      <c r="B238" s="2" t="n">
+        <v>43780</v>
       </c>
       <c r="C238" t="n">
         <v>140221</v>
@@ -12165,8 +12169,8 @@
       <c r="A239" s="1" t="n">
         <v>237</v>
       </c>
-      <c r="B239" t="n">
-        <v>20191111</v>
+      <c r="B239" s="2" t="n">
+        <v>43780</v>
       </c>
       <c r="C239" t="n">
         <v>165049</v>
@@ -12217,8 +12221,8 @@
       <c r="A240" s="1" t="n">
         <v>238</v>
       </c>
-      <c r="B240" t="n">
-        <v>20191112</v>
+      <c r="B240" s="2" t="n">
+        <v>43781</v>
       </c>
       <c r="C240" t="n">
         <v>3003</v>
@@ -12261,8 +12265,8 @@
       <c r="A241" s="1" t="n">
         <v>239</v>
       </c>
-      <c r="B241" t="n">
-        <v>20191118</v>
+      <c r="B241" s="2" t="n">
+        <v>43787</v>
       </c>
       <c r="C241" t="n">
         <v>135109</v>
@@ -12313,8 +12317,8 @@
       <c r="A242" s="1" t="n">
         <v>240</v>
       </c>
-      <c r="B242" t="n">
-        <v>20191118</v>
+      <c r="B242" s="2" t="n">
+        <v>43787</v>
       </c>
       <c r="C242" t="n">
         <v>144339</v>
@@ -12365,8 +12369,8 @@
       <c r="A243" s="1" t="n">
         <v>241</v>
       </c>
-      <c r="B243" t="n">
-        <v>20191120</v>
+      <c r="B243" s="2" t="n">
+        <v>43789</v>
       </c>
       <c r="C243" t="n">
         <v>121905</v>
@@ -12417,8 +12421,8 @@
       <c r="A244" s="1" t="n">
         <v>242</v>
       </c>
-      <c r="B244" t="n">
-        <v>20191202</v>
+      <c r="B244" s="2" t="n">
+        <v>43801</v>
       </c>
       <c r="C244" t="n">
         <v>40029</v>
@@ -12461,8 +12465,8 @@
       <c r="A245" s="1" t="n">
         <v>243</v>
       </c>
-      <c r="B245" t="n">
-        <v>20191202</v>
+      <c r="B245" s="2" t="n">
+        <v>43801</v>
       </c>
       <c r="C245" t="n">
         <v>40903</v>
@@ -12505,8 +12509,8 @@
       <c r="A246" s="1" t="n">
         <v>244</v>
       </c>
-      <c r="B246" t="n">
-        <v>20191202</v>
+      <c r="B246" s="2" t="n">
+        <v>43801</v>
       </c>
       <c r="C246" t="n">
         <v>43317</v>
@@ -12549,8 +12553,8 @@
       <c r="A247" s="1" t="n">
         <v>245</v>
       </c>
-      <c r="B247" t="n">
-        <v>20191202</v>
+      <c r="B247" s="2" t="n">
+        <v>43801</v>
       </c>
       <c r="C247" t="n">
         <v>162839</v>
@@ -12601,8 +12605,8 @@
       <c r="A248" s="1" t="n">
         <v>246</v>
       </c>
-      <c r="B248" t="n">
-        <v>20191202</v>
+      <c r="B248" s="2" t="n">
+        <v>43801</v>
       </c>
       <c r="C248" t="n">
         <v>163505</v>
@@ -12653,8 +12657,8 @@
       <c r="A249" s="1" t="n">
         <v>247</v>
       </c>
-      <c r="B249" t="n">
-        <v>20191203</v>
+      <c r="B249" s="2" t="n">
+        <v>43802</v>
       </c>
       <c r="C249" t="n">
         <v>162802</v>
@@ -12705,8 +12709,8 @@
       <c r="A250" s="1" t="n">
         <v>248</v>
       </c>
-      <c r="B250" t="n">
-        <v>20191210</v>
+      <c r="B250" s="2" t="n">
+        <v>43809</v>
       </c>
       <c r="C250" t="n">
         <v>121147</v>
@@ -12757,8 +12761,8 @@
       <c r="A251" s="1" t="n">
         <v>249</v>
       </c>
-      <c r="B251" t="n">
-        <v>20191210</v>
+      <c r="B251" s="2" t="n">
+        <v>43809</v>
       </c>
       <c r="C251" t="n">
         <v>150132</v>
@@ -12805,8 +12809,8 @@
       <c r="A252" s="1" t="n">
         <v>250</v>
       </c>
-      <c r="B252" t="n">
-        <v>20191210</v>
+      <c r="B252" s="2" t="n">
+        <v>43809</v>
       </c>
       <c r="C252" t="n">
         <v>150519</v>
@@ -12849,8 +12853,8 @@
       <c r="A253" s="1" t="n">
         <v>251</v>
       </c>
-      <c r="B253" t="n">
-        <v>20191210</v>
+      <c r="B253" s="2" t="n">
+        <v>43809</v>
       </c>
       <c r="C253" t="n">
         <v>152535</v>
@@ -12893,8 +12897,8 @@
       <c r="A254" s="1" t="n">
         <v>252</v>
       </c>
-      <c r="B254" t="n">
-        <v>20191210</v>
+      <c r="B254" s="2" t="n">
+        <v>43809</v>
       </c>
       <c r="C254" t="n">
         <v>152541</v>
@@ -12937,8 +12941,8 @@
       <c r="A255" s="1" t="n">
         <v>253</v>
       </c>
-      <c r="B255" t="n">
-        <v>20191210</v>
+      <c r="B255" s="2" t="n">
+        <v>43809</v>
       </c>
       <c r="C255" t="n">
         <v>152627</v>
@@ -12989,8 +12993,8 @@
       <c r="A256" s="1" t="n">
         <v>254</v>
       </c>
-      <c r="B256" t="n">
-        <v>20191210</v>
+      <c r="B256" s="2" t="n">
+        <v>43809</v>
       </c>
       <c r="C256" t="n">
         <v>152627</v>
@@ -13041,8 +13045,8 @@
       <c r="A257" s="1" t="n">
         <v>255</v>
       </c>
-      <c r="B257" t="n">
-        <v>20191210</v>
+      <c r="B257" s="2" t="n">
+        <v>43809</v>
       </c>
       <c r="C257" t="n">
         <v>152627</v>
@@ -13093,8 +13097,8 @@
       <c r="A258" s="1" t="n">
         <v>256</v>
       </c>
-      <c r="B258" t="n">
-        <v>20191210</v>
+      <c r="B258" s="2" t="n">
+        <v>43809</v>
       </c>
       <c r="C258" t="n">
         <v>152627</v>
@@ -13145,8 +13149,8 @@
       <c r="A259" s="1" t="n">
         <v>257</v>
       </c>
-      <c r="B259" t="n">
-        <v>20191210</v>
+      <c r="B259" s="2" t="n">
+        <v>43809</v>
       </c>
       <c r="C259" t="n">
         <v>152627</v>
@@ -13197,8 +13201,8 @@
       <c r="A260" s="1" t="n">
         <v>258</v>
       </c>
-      <c r="B260" t="n">
-        <v>20191210</v>
+      <c r="B260" s="2" t="n">
+        <v>43809</v>
       </c>
       <c r="C260" t="n">
         <v>152627</v>
@@ -13249,8 +13253,8 @@
       <c r="A261" s="1" t="n">
         <v>259</v>
       </c>
-      <c r="B261" t="n">
-        <v>20191211</v>
+      <c r="B261" s="2" t="n">
+        <v>43810</v>
       </c>
       <c r="C261" t="n">
         <v>1251</v>
@@ -13293,8 +13297,8 @@
       <c r="A262" s="1" t="n">
         <v>260</v>
       </c>
-      <c r="B262" t="n">
-        <v>20191212</v>
+      <c r="B262" s="2" t="n">
+        <v>43811</v>
       </c>
       <c r="C262" t="n">
         <v>151005</v>
@@ -13345,8 +13349,8 @@
       <c r="A263" s="1" t="n">
         <v>261</v>
       </c>
-      <c r="B263" t="n">
-        <v>20191221</v>
+      <c r="B263" s="2" t="n">
+        <v>43820</v>
       </c>
       <c r="C263" t="n">
         <v>30144</v>
@@ -13389,8 +13393,8 @@
       <c r="A264" s="1" t="n">
         <v>262</v>
       </c>
-      <c r="B264" t="n">
-        <v>20191227</v>
+      <c r="B264" s="2" t="n">
+        <v>43826</v>
       </c>
       <c r="C264" t="n">
         <v>160828</v>
@@ -13441,8 +13445,8 @@
       <c r="A265" s="1" t="n">
         <v>263</v>
       </c>
-      <c r="B265" t="n">
-        <v>20191227</v>
+      <c r="B265" s="2" t="n">
+        <v>43826</v>
       </c>
       <c r="C265" t="n">
         <v>164823</v>
@@ -13493,8 +13497,8 @@
       <c r="A266" s="1" t="n">
         <v>264</v>
       </c>
-      <c r="B266" t="n">
-        <v>20191227</v>
+      <c r="B266" s="2" t="n">
+        <v>43826</v>
       </c>
       <c r="C266" t="n">
         <v>164823</v>
@@ -13545,8 +13549,8 @@
       <c r="A267" s="1" t="n">
         <v>265</v>
       </c>
-      <c r="B267" t="n">
-        <v>20200102</v>
+      <c r="B267" s="2" t="n">
+        <v>43832</v>
       </c>
       <c r="C267" t="n">
         <v>35124</v>
@@ -13589,8 +13593,8 @@
       <c r="A268" s="1" t="n">
         <v>266</v>
       </c>
-      <c r="B268" t="n">
-        <v>20200102</v>
+      <c r="B268" s="2" t="n">
+        <v>43832</v>
       </c>
       <c r="C268" t="n">
         <v>35414</v>
@@ -13633,8 +13637,8 @@
       <c r="A269" s="1" t="n">
         <v>267</v>
       </c>
-      <c r="B269" t="n">
-        <v>20200102</v>
+      <c r="B269" s="2" t="n">
+        <v>43832</v>
       </c>
       <c r="C269" t="n">
         <v>42413</v>
@@ -13677,8 +13681,8 @@
       <c r="A270" s="1" t="n">
         <v>268</v>
       </c>
-      <c r="B270" t="n">
-        <v>20200106</v>
+      <c r="B270" s="2" t="n">
+        <v>43836</v>
       </c>
       <c r="C270" t="n">
         <v>154823</v>
@@ -13725,8 +13729,8 @@
       <c r="A271" s="1" t="n">
         <v>269</v>
       </c>
-      <c r="B271" t="n">
-        <v>20200110</v>
+      <c r="B271" s="2" t="n">
+        <v>43840</v>
       </c>
       <c r="C271" t="n">
         <v>130643</v>
@@ -13777,8 +13781,8 @@
       <c r="A272" s="1" t="n">
         <v>270</v>
       </c>
-      <c r="B272" t="n">
-        <v>20200110</v>
+      <c r="B272" s="2" t="n">
+        <v>43840</v>
       </c>
       <c r="C272" t="n">
         <v>131424</v>
@@ -13829,8 +13833,8 @@
       <c r="A273" s="1" t="n">
         <v>271</v>
       </c>
-      <c r="B273" t="n">
-        <v>20200110</v>
+      <c r="B273" s="2" t="n">
+        <v>43840</v>
       </c>
       <c r="C273" t="n">
         <v>162629</v>
@@ -13873,8 +13877,8 @@
       <c r="A274" s="1" t="n">
         <v>272</v>
       </c>
-      <c r="B274" t="n">
-        <v>20200110</v>
+      <c r="B274" s="2" t="n">
+        <v>43840</v>
       </c>
       <c r="C274" t="n">
         <v>162636</v>
@@ -13917,8 +13921,8 @@
       <c r="A275" s="1" t="n">
         <v>273</v>
       </c>
-      <c r="B275" t="n">
-        <v>20200110</v>
+      <c r="B275" s="2" t="n">
+        <v>43840</v>
       </c>
       <c r="C275" t="n">
         <v>162724</v>
@@ -13969,8 +13973,8 @@
       <c r="A276" s="1" t="n">
         <v>274</v>
       </c>
-      <c r="B276" t="n">
-        <v>20200110</v>
+      <c r="B276" s="2" t="n">
+        <v>43840</v>
       </c>
       <c r="C276" t="n">
         <v>162725</v>
@@ -14021,8 +14025,8 @@
       <c r="A277" s="1" t="n">
         <v>275</v>
       </c>
-      <c r="B277" t="n">
-        <v>20200110</v>
+      <c r="B277" s="2" t="n">
+        <v>43840</v>
       </c>
       <c r="C277" t="n">
         <v>162725</v>
@@ -14073,8 +14077,8 @@
       <c r="A278" s="1" t="n">
         <v>276</v>
       </c>
-      <c r="B278" t="n">
-        <v>20200110</v>
+      <c r="B278" s="2" t="n">
+        <v>43840</v>
       </c>
       <c r="C278" t="n">
         <v>162725</v>
@@ -14125,8 +14129,8 @@
       <c r="A279" s="1" t="n">
         <v>277</v>
       </c>
-      <c r="B279" t="n">
-        <v>20200110</v>
+      <c r="B279" s="2" t="n">
+        <v>43840</v>
       </c>
       <c r="C279" t="n">
         <v>162725</v>
@@ -14177,8 +14181,8 @@
       <c r="A280" s="1" t="n">
         <v>278</v>
       </c>
-      <c r="B280" t="n">
-        <v>20200110</v>
+      <c r="B280" s="2" t="n">
+        <v>43840</v>
       </c>
       <c r="C280" t="n">
         <v>162725</v>
@@ -14229,8 +14233,8 @@
       <c r="A281" s="1" t="n">
         <v>279</v>
       </c>
-      <c r="B281" t="n">
-        <v>20200113</v>
+      <c r="B281" s="2" t="n">
+        <v>43843</v>
       </c>
       <c r="C281" t="n">
         <v>4023</v>
@@ -14273,8 +14277,8 @@
       <c r="A282" s="1" t="n">
         <v>280</v>
       </c>
-      <c r="B282" t="n">
-        <v>20200113</v>
+      <c r="B282" s="2" t="n">
+        <v>43843</v>
       </c>
       <c r="C282" t="n">
         <v>94328</v>
@@ -14321,8 +14325,8 @@
       <c r="A283" s="1" t="n">
         <v>281</v>
       </c>
-      <c r="B283" t="n">
-        <v>20200113</v>
+      <c r="B283" s="2" t="n">
+        <v>43843</v>
       </c>
       <c r="C283" t="n">
         <v>94831</v>
@@ -14365,8 +14369,8 @@
       <c r="A284" s="1" t="n">
         <v>282</v>
       </c>
-      <c r="B284" t="n">
-        <v>20200119</v>
+      <c r="B284" s="2" t="n">
+        <v>43849</v>
       </c>
       <c r="C284" t="n">
         <v>170944</v>
@@ -14417,8 +14421,8 @@
       <c r="A285" s="1" t="n">
         <v>283</v>
       </c>
-      <c r="B285" t="n">
-        <v>20200119</v>
+      <c r="B285" s="2" t="n">
+        <v>43849</v>
       </c>
       <c r="C285" t="n">
         <v>171456</v>
@@ -14469,8 +14473,8 @@
       <c r="A286" s="1" t="n">
         <v>284</v>
       </c>
-      <c r="B286" t="n">
-        <v>20200119</v>
+      <c r="B286" s="2" t="n">
+        <v>43849</v>
       </c>
       <c r="C286" t="n">
         <v>171456</v>
@@ -14521,8 +14525,8 @@
       <c r="A287" s="1" t="n">
         <v>285</v>
       </c>
-      <c r="B287" t="n">
-        <v>20200202</v>
+      <c r="B287" s="2" t="n">
+        <v>43863</v>
       </c>
       <c r="C287" t="n">
         <v>35507</v>
@@ -14565,8 +14569,8 @@
       <c r="A288" s="1" t="n">
         <v>286</v>
       </c>
-      <c r="B288" t="n">
-        <v>20200202</v>
+      <c r="B288" s="2" t="n">
+        <v>43863</v>
       </c>
       <c r="C288" t="n">
         <v>35508</v>
@@ -14609,8 +14613,8 @@
       <c r="A289" s="1" t="n">
         <v>287</v>
       </c>
-      <c r="B289" t="n">
-        <v>20200202</v>
+      <c r="B289" s="2" t="n">
+        <v>43863</v>
       </c>
       <c r="C289" t="n">
         <v>40915</v>
@@ -14653,8 +14657,8 @@
       <c r="A290" s="1" t="n">
         <v>288</v>
       </c>
-      <c r="B290" t="n">
-        <v>20200210</v>
+      <c r="B290" s="2" t="n">
+        <v>43871</v>
       </c>
       <c r="C290" t="n">
         <v>144116</v>
@@ -14705,8 +14709,8 @@
       <c r="A291" s="1" t="n">
         <v>289</v>
       </c>
-      <c r="B291" t="n">
-        <v>20200210</v>
+      <c r="B291" s="2" t="n">
+        <v>43871</v>
       </c>
       <c r="C291" t="n">
         <v>154456</v>
@@ -14757,8 +14761,8 @@
       <c r="A292" s="1" t="n">
         <v>290</v>
       </c>
-      <c r="B292" t="n">
-        <v>20200210</v>
+      <c r="B292" s="2" t="n">
+        <v>43871</v>
       </c>
       <c r="C292" t="n">
         <v>154522</v>
@@ -14801,8 +14805,8 @@
       <c r="A293" s="1" t="n">
         <v>291</v>
       </c>
-      <c r="B293" t="n">
-        <v>20200210</v>
+      <c r="B293" s="2" t="n">
+        <v>43871</v>
       </c>
       <c r="C293" t="n">
         <v>154528</v>
@@ -14845,8 +14849,8 @@
       <c r="A294" s="1" t="n">
         <v>292</v>
       </c>
-      <c r="B294" t="n">
-        <v>20200211</v>
+      <c r="B294" s="2" t="n">
+        <v>43872</v>
       </c>
       <c r="C294" t="n">
         <v>4812</v>
@@ -14889,8 +14893,8 @@
       <c r="A295" s="1" t="n">
         <v>293</v>
       </c>
-      <c r="B295" t="n">
-        <v>20200218</v>
+      <c r="B295" s="2" t="n">
+        <v>43879</v>
       </c>
       <c r="C295" t="n">
         <v>102926</v>
@@ -14933,8 +14937,8 @@
       <c r="A296" s="1" t="n">
         <v>294</v>
       </c>
-      <c r="B296" t="n">
-        <v>20200218</v>
+      <c r="B296" s="2" t="n">
+        <v>43879</v>
       </c>
       <c r="C296" t="n">
         <v>110202</v>
@@ -14981,8 +14985,8 @@
       <c r="A297" s="1" t="n">
         <v>295</v>
       </c>
-      <c r="B297" t="n">
-        <v>20200227</v>
+      <c r="B297" s="2" t="n">
+        <v>43888</v>
       </c>
       <c r="C297" t="n">
         <v>102438</v>
@@ -15033,8 +15037,8 @@
       <c r="A298" s="1" t="n">
         <v>296</v>
       </c>
-      <c r="B298" t="n">
-        <v>20200228</v>
+      <c r="B298" s="2" t="n">
+        <v>43889</v>
       </c>
       <c r="C298" t="n">
         <v>141431</v>
@@ -15085,8 +15089,8 @@
       <c r="A299" s="1" t="n">
         <v>297</v>
       </c>
-      <c r="B299" t="n">
-        <v>20200228</v>
+      <c r="B299" s="2" t="n">
+        <v>43889</v>
       </c>
       <c r="C299" t="n">
         <v>142442</v>
@@ -15137,8 +15141,8 @@
       <c r="A300" s="1" t="n">
         <v>298</v>
       </c>
-      <c r="B300" t="n">
-        <v>20200228</v>
+      <c r="B300" s="2" t="n">
+        <v>43889</v>
       </c>
       <c r="C300" t="n">
         <v>160933</v>
@@ -15189,8 +15193,8 @@
       <c r="A301" s="1" t="n">
         <v>299</v>
       </c>
-      <c r="B301" t="n">
-        <v>20200228</v>
+      <c r="B301" s="2" t="n">
+        <v>43889</v>
       </c>
       <c r="C301" t="n">
         <v>162339</v>
@@ -15241,8 +15245,8 @@
       <c r="A302" s="1" t="n">
         <v>300</v>
       </c>
-      <c r="B302" t="n">
-        <v>20200302</v>
+      <c r="B302" s="2" t="n">
+        <v>43892</v>
       </c>
       <c r="C302" t="n">
         <v>40239</v>
@@ -15285,8 +15289,8 @@
       <c r="A303" s="1" t="n">
         <v>301</v>
       </c>
-      <c r="B303" t="n">
-        <v>20200302</v>
+      <c r="B303" s="2" t="n">
+        <v>43892</v>
       </c>
       <c r="C303" t="n">
         <v>43028</v>
@@ -15329,8 +15333,8 @@
       <c r="A304" s="1" t="n">
         <v>302</v>
       </c>
-      <c r="B304" t="n">
-        <v>20200303</v>
+      <c r="B304" s="2" t="n">
+        <v>43893</v>
       </c>
       <c r="C304" t="n">
         <v>162131</v>

</xml_diff>